<commit_message>
add try and except line 15 - 20
</commit_message>
<xml_diff>
--- a/2024-04-19_Daily_Check_list.xlsx
+++ b/2024-04-19_Daily_Check_list.xlsx
@@ -6949,18 +6949,111 @@
           <t>2024-04-19 16:39:01</t>
         </is>
       </c>
-      <c r="F6" s="38" t="n"/>
-      <c r="G6" s="38" t="n"/>
-      <c r="H6" s="38" t="n"/>
-      <c r="I6" s="38" t="n"/>
-      <c r="J6" s="38" t="n"/>
-      <c r="K6" s="38" t="n"/>
-      <c r="L6" s="38" t="n"/>
-      <c r="M6" s="38" t="n"/>
-      <c r="N6" s="38" t="n"/>
-      <c r="O6" s="38" t="n"/>
-      <c r="P6" s="38" t="n"/>
-      <c r="Q6" s="38" t="n"/>
+      <c r="F6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:18:43</t>
+        </is>
+      </c>
+      <c r="G6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:20:24</t>
+        </is>
+      </c>
+      <c r="H6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:31:09</t>
+        </is>
+      </c>
+      <c r="I6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:41:10</t>
+        </is>
+      </c>
+      <c r="J6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:51:12</t>
+        </is>
+      </c>
+      <c r="K6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 18:11:14</t>
+        </is>
+      </c>
+      <c r="L6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 18:21:16</t>
+        </is>
+      </c>
+      <c r="M6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 18:31:17</t>
+        </is>
+      </c>
+      <c r="N6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 18:41:19</t>
+        </is>
+      </c>
+      <c r="O6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 18:51:21</t>
+        </is>
+      </c>
+      <c r="P6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:01:46</t>
+        </is>
+      </c>
+      <c r="Q6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:11:48</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:21:49</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:31:51</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:41:53</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2024-04-19 21:51:54</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>2024-04-19 22:01:56</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>2024-04-19 22:11:58</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>2024-04-19 22:21:59</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2024-04-19 22:32:01</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>2024-04-19 22:42:03</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="15.65" customHeight="1">
       <c r="A7" s="16" t="inlineStr">
@@ -6988,18 +7081,111 @@
           <t>22005.00</t>
         </is>
       </c>
-      <c r="F7" s="39" t="n"/>
-      <c r="G7" s="39" t="n"/>
-      <c r="H7" s="39" t="n"/>
-      <c r="I7" s="39" t="n"/>
-      <c r="J7" s="39" t="n"/>
-      <c r="K7" s="39" t="n"/>
-      <c r="L7" s="39" t="n"/>
-      <c r="M7" s="39" t="n"/>
-      <c r="N7" s="39" t="n"/>
-      <c r="O7" s="39" t="n"/>
-      <c r="P7" s="39" t="n"/>
-      <c r="Q7" s="39" t="n"/>
+      <c r="F7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="G7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="H7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="I7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="J7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="K7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="L7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="M7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="N7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="O7" s="39" t="inlineStr">
+        <is>
+          <t>22005.00</t>
+        </is>
+      </c>
+      <c r="P7" s="39" t="inlineStr">
+        <is>
+          <t>22007.00</t>
+        </is>
+      </c>
+      <c r="Q7" s="39" t="inlineStr">
+        <is>
+          <t>22007.00</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>22007.00</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>22007.00</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>22008.00</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15.65" customHeight="1">
       <c r="A8" s="11" t="inlineStr">
@@ -7027,18 +7213,111 @@
           <t>440.81</t>
         </is>
       </c>
-      <c r="F8" s="40" t="n"/>
-      <c r="G8" s="40" t="n"/>
-      <c r="H8" s="40" t="n"/>
-      <c r="I8" s="41" t="n"/>
-      <c r="J8" s="42" t="n"/>
-      <c r="K8" s="42" t="n"/>
-      <c r="L8" s="40" t="n"/>
-      <c r="M8" s="40" t="n"/>
-      <c r="N8" s="42" t="n"/>
-      <c r="O8" s="42" t="n"/>
-      <c r="P8" s="42" t="n"/>
-      <c r="Q8" s="41" t="n"/>
+      <c r="F8" s="40" t="inlineStr">
+        <is>
+          <t>440.38</t>
+        </is>
+      </c>
+      <c r="G8" s="40" t="inlineStr">
+        <is>
+          <t>440.52</t>
+        </is>
+      </c>
+      <c r="H8" s="40" t="inlineStr">
+        <is>
+          <t>440.38</t>
+        </is>
+      </c>
+      <c r="I8" s="41" t="inlineStr">
+        <is>
+          <t>440.38</t>
+        </is>
+      </c>
+      <c r="J8" s="42" t="inlineStr">
+        <is>
+          <t>440.09</t>
+        </is>
+      </c>
+      <c r="K8" s="42" t="inlineStr">
+        <is>
+          <t>438.93</t>
+        </is>
+      </c>
+      <c r="L8" s="40" t="inlineStr">
+        <is>
+          <t>439.22</t>
+        </is>
+      </c>
+      <c r="M8" s="40" t="inlineStr">
+        <is>
+          <t>439.08</t>
+        </is>
+      </c>
+      <c r="N8" s="42" t="inlineStr">
+        <is>
+          <t>439.08</t>
+        </is>
+      </c>
+      <c r="O8" s="42" t="inlineStr">
+        <is>
+          <t>439.08</t>
+        </is>
+      </c>
+      <c r="P8" s="42" t="inlineStr">
+        <is>
+          <t>484.79</t>
+        </is>
+      </c>
+      <c r="Q8" s="41" t="inlineStr">
+        <is>
+          <t>485.23</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>486.09</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>484.21</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>485.95</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>475.10</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>473.80</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>473.36</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>472.93</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>472.49</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>472.35</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15.65" customHeight="1">
       <c r="A9" s="11" t="inlineStr">
@@ -7066,18 +7345,111 @@
           <t>441.74</t>
         </is>
       </c>
-      <c r="F9" s="43" t="n"/>
-      <c r="G9" s="43" t="n"/>
-      <c r="H9" s="43" t="n"/>
-      <c r="I9" s="44" t="n"/>
-      <c r="J9" s="42" t="n"/>
-      <c r="K9" s="42" t="n"/>
-      <c r="L9" s="45" t="n"/>
-      <c r="M9" s="43" t="n"/>
-      <c r="N9" s="46" t="n"/>
-      <c r="O9" s="42" t="n"/>
-      <c r="P9" s="42" t="n"/>
-      <c r="Q9" s="44" t="n"/>
+      <c r="F9" s="43" t="inlineStr">
+        <is>
+          <t>440.44</t>
+        </is>
+      </c>
+      <c r="G9" s="43" t="inlineStr">
+        <is>
+          <t>440.73</t>
+        </is>
+      </c>
+      <c r="H9" s="43" t="inlineStr">
+        <is>
+          <t>440.44</t>
+        </is>
+      </c>
+      <c r="I9" s="44" t="inlineStr">
+        <is>
+          <t>440.59</t>
+        </is>
+      </c>
+      <c r="J9" s="42" t="inlineStr">
+        <is>
+          <t>440.01</t>
+        </is>
+      </c>
+      <c r="K9" s="42" t="inlineStr">
+        <is>
+          <t>439.28</t>
+        </is>
+      </c>
+      <c r="L9" s="45" t="inlineStr">
+        <is>
+          <t>439.86</t>
+        </is>
+      </c>
+      <c r="M9" s="43" t="inlineStr">
+        <is>
+          <t>439.14</t>
+        </is>
+      </c>
+      <c r="N9" s="46" t="inlineStr">
+        <is>
+          <t>439.57</t>
+        </is>
+      </c>
+      <c r="O9" s="42" t="inlineStr">
+        <is>
+          <t>439.14</t>
+        </is>
+      </c>
+      <c r="P9" s="42" t="inlineStr">
+        <is>
+          <t>1203.69</t>
+        </is>
+      </c>
+      <c r="Q9" s="44" t="inlineStr">
+        <is>
+          <t>1218.45</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>1234.80</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>1241.45</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>1257.80</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>475.17</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>474.01</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>473.58</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>473.29</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>472.27</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>472.42</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15.65" customHeight="1">
       <c r="A10" s="11" t="inlineStr">
@@ -7105,18 +7477,111 @@
           <t>3097.64</t>
         </is>
       </c>
-      <c r="F10" s="47" t="n"/>
-      <c r="G10" s="47" t="n"/>
-      <c r="H10" s="47" t="n"/>
-      <c r="I10" s="44" t="n"/>
-      <c r="J10" s="42" t="n"/>
-      <c r="K10" s="42" t="n"/>
-      <c r="L10" s="45" t="n"/>
-      <c r="M10" s="47" t="n"/>
-      <c r="N10" s="46" t="n"/>
-      <c r="O10" s="42" t="n"/>
-      <c r="P10" s="42" t="n"/>
-      <c r="Q10" s="44" t="n"/>
+      <c r="F10" s="47" t="inlineStr">
+        <is>
+          <t>3070.16</t>
+        </is>
+      </c>
+      <c r="G10" s="47" t="inlineStr">
+        <is>
+          <t>3068.86</t>
+        </is>
+      </c>
+      <c r="H10" s="47" t="inlineStr">
+        <is>
+          <t>3061.19</t>
+        </is>
+      </c>
+      <c r="I10" s="44" t="inlineStr">
+        <is>
+          <t>3052.36</t>
+        </is>
+      </c>
+      <c r="J10" s="42" t="inlineStr">
+        <is>
+          <t>3043.83</t>
+        </is>
+      </c>
+      <c r="K10" s="42" t="inlineStr">
+        <is>
+          <t>3026.76</t>
+        </is>
+      </c>
+      <c r="L10" s="45" t="inlineStr">
+        <is>
+          <t>3016.64</t>
+        </is>
+      </c>
+      <c r="M10" s="47" t="inlineStr">
+        <is>
+          <t>3006.51</t>
+        </is>
+      </c>
+      <c r="N10" s="46" t="inlineStr">
+        <is>
+          <t>2997.83</t>
+        </is>
+      </c>
+      <c r="O10" s="42" t="inlineStr">
+        <is>
+          <t>2988.72</t>
+        </is>
+      </c>
+      <c r="P10" s="42" t="inlineStr">
+        <is>
+          <t>2538.98</t>
+        </is>
+      </c>
+      <c r="Q10" s="44" t="inlineStr">
+        <is>
+          <t>2754.95</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>2982.64</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>3219.88</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>3475.48</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>3391.73</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>3335.74</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>3292.35</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>3258.35</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>3234.49</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>3214.96</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15.65" customHeight="1">
       <c r="A11" s="11" t="inlineStr">
@@ -7144,18 +7609,111 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="F11" s="47" t="n"/>
-      <c r="G11" s="47" t="n"/>
-      <c r="H11" s="47" t="n"/>
-      <c r="I11" s="44" t="n"/>
-      <c r="J11" s="42" t="n"/>
-      <c r="K11" s="42" t="n"/>
-      <c r="L11" s="45" t="n"/>
-      <c r="M11" s="47" t="n"/>
-      <c r="N11" s="46" t="n"/>
-      <c r="O11" s="42" t="n"/>
-      <c r="P11" s="42" t="n"/>
-      <c r="Q11" s="44" t="n"/>
+      <c r="F11" s="47" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="G11" s="47" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="H11" s="47" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="I11" s="44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="J11" s="42" t="inlineStr">
+        <is>
+          <t>-0.29</t>
+        </is>
+      </c>
+      <c r="K11" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L11" s="45" t="inlineStr">
+        <is>
+          <t>-0.29</t>
+        </is>
+      </c>
+      <c r="M11" s="47" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="N11" s="46" t="inlineStr">
+        <is>
+          <t>-0.43</t>
+        </is>
+      </c>
+      <c r="O11" s="42" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="P11" s="42" t="inlineStr">
+        <is>
+          <t>43.84</t>
+        </is>
+      </c>
+      <c r="Q11" s="44" t="inlineStr">
+        <is>
+          <t>44.42</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>44.42</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>44.56</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>44.13</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>-0.29</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>-0.29</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>-0.29</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15.65" customHeight="1">
       <c r="A12" s="11" t="inlineStr">
@@ -7183,18 +7741,111 @@
           <t>47.36</t>
         </is>
       </c>
-      <c r="F12" s="42" t="n"/>
-      <c r="G12" s="42" t="n"/>
-      <c r="H12" s="42" t="n"/>
-      <c r="I12" s="44" t="n"/>
-      <c r="J12" s="42" t="n"/>
-      <c r="K12" s="42" t="n"/>
-      <c r="L12" s="45" t="n"/>
-      <c r="M12" s="42" t="n"/>
-      <c r="N12" s="46" t="n"/>
-      <c r="O12" s="42" t="n"/>
-      <c r="P12" s="42" t="n"/>
-      <c r="Q12" s="44" t="n"/>
+      <c r="F12" s="42" t="inlineStr">
+        <is>
+          <t>43.83</t>
+        </is>
+      </c>
+      <c r="G12" s="42" t="inlineStr">
+        <is>
+          <t>43.74</t>
+        </is>
+      </c>
+      <c r="H12" s="42" t="inlineStr">
+        <is>
+          <t>43.00</t>
+        </is>
+      </c>
+      <c r="I12" s="44" t="inlineStr">
+        <is>
+          <t>42.33</t>
+        </is>
+      </c>
+      <c r="J12" s="42" t="inlineStr">
+        <is>
+          <t>41.75</t>
+        </is>
+      </c>
+      <c r="K12" s="42" t="inlineStr">
+        <is>
+          <t>40.60</t>
+        </is>
+      </c>
+      <c r="L12" s="45" t="inlineStr">
+        <is>
+          <t>40.11</t>
+        </is>
+      </c>
+      <c r="M12" s="42" t="inlineStr">
+        <is>
+          <t>39.63</t>
+        </is>
+      </c>
+      <c r="N12" s="46" t="inlineStr">
+        <is>
+          <t>39.16</t>
+        </is>
+      </c>
+      <c r="O12" s="42" t="inlineStr">
+        <is>
+          <t>38.69</t>
+        </is>
+      </c>
+      <c r="P12" s="42" t="inlineStr">
+        <is>
+          <t>96.04</t>
+        </is>
+      </c>
+      <c r="Q12" s="44" t="inlineStr">
+        <is>
+          <t>97.10</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>98.67</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>100.07</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>101.84</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>91.31</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>81.96</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>74.75</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>69.04</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>64.15</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>60.20</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="15.65" customHeight="1">
       <c r="A13" s="11" t="inlineStr">
@@ -7222,18 +7873,111 @@
           <t>48.32</t>
         </is>
       </c>
-      <c r="F13" s="42" t="n"/>
-      <c r="G13" s="42" t="n"/>
-      <c r="H13" s="42" t="n"/>
-      <c r="I13" s="44" t="n"/>
-      <c r="J13" s="42" t="n"/>
-      <c r="K13" s="42" t="n"/>
-      <c r="L13" s="42" t="n"/>
-      <c r="M13" s="42" t="n"/>
-      <c r="N13" s="42" t="n"/>
-      <c r="O13" s="42" t="n"/>
-      <c r="P13" s="42" t="n"/>
-      <c r="Q13" s="44" t="n"/>
+      <c r="F13" s="42" t="inlineStr">
+        <is>
+          <t>44.53</t>
+        </is>
+      </c>
+      <c r="G13" s="42" t="inlineStr">
+        <is>
+          <t>44.40</t>
+        </is>
+      </c>
+      <c r="H13" s="42" t="inlineStr">
+        <is>
+          <t>43.67</t>
+        </is>
+      </c>
+      <c r="I13" s="44" t="inlineStr">
+        <is>
+          <t>42.96</t>
+        </is>
+      </c>
+      <c r="J13" s="42" t="inlineStr">
+        <is>
+          <t>42.38</t>
+        </is>
+      </c>
+      <c r="K13" s="42" t="inlineStr">
+        <is>
+          <t>41.34</t>
+        </is>
+      </c>
+      <c r="L13" s="42" t="inlineStr">
+        <is>
+          <t>40.87</t>
+        </is>
+      </c>
+      <c r="M13" s="42" t="inlineStr">
+        <is>
+          <t>40.41</t>
+        </is>
+      </c>
+      <c r="N13" s="42" t="inlineStr">
+        <is>
+          <t>39.97</t>
+        </is>
+      </c>
+      <c r="O13" s="42" t="inlineStr">
+        <is>
+          <t>39.61</t>
+        </is>
+      </c>
+      <c r="P13" s="42" t="inlineStr">
+        <is>
+          <t>99.05</t>
+        </is>
+      </c>
+      <c r="Q13" s="44" t="inlineStr">
+        <is>
+          <t>100.32</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>101.87</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>103.44</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>104.75</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>93.89</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>84.70</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>77.52</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>71.49</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>66.57</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>62.45</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15.65" customHeight="1">
       <c r="A14" s="11" t="inlineStr">
@@ -7261,18 +8005,111 @@
           <t>47.06</t>
         </is>
       </c>
-      <c r="F14" s="42" t="n"/>
-      <c r="G14" s="42" t="n"/>
-      <c r="H14" s="42" t="n"/>
-      <c r="I14" s="44" t="n"/>
-      <c r="J14" s="42" t="n"/>
-      <c r="K14" s="42" t="n"/>
-      <c r="L14" s="42" t="n"/>
-      <c r="M14" s="42" t="n"/>
-      <c r="N14" s="42" t="n"/>
-      <c r="O14" s="42" t="n"/>
-      <c r="P14" s="42" t="n"/>
-      <c r="Q14" s="44" t="n"/>
+      <c r="F14" s="42" t="inlineStr">
+        <is>
+          <t>42.74</t>
+        </is>
+      </c>
+      <c r="G14" s="42" t="inlineStr">
+        <is>
+          <t>42.60</t>
+        </is>
+      </c>
+      <c r="H14" s="42" t="inlineStr">
+        <is>
+          <t>41.79</t>
+        </is>
+      </c>
+      <c r="I14" s="44" t="inlineStr">
+        <is>
+          <t>41.01</t>
+        </is>
+      </c>
+      <c r="J14" s="42" t="inlineStr">
+        <is>
+          <t>40.38</t>
+        </is>
+      </c>
+      <c r="K14" s="42" t="inlineStr">
+        <is>
+          <t>39.26</t>
+        </is>
+      </c>
+      <c r="L14" s="42" t="inlineStr">
+        <is>
+          <t>38.70</t>
+        </is>
+      </c>
+      <c r="M14" s="42" t="inlineStr">
+        <is>
+          <t>38.19</t>
+        </is>
+      </c>
+      <c r="N14" s="42" t="inlineStr">
+        <is>
+          <t>37.68</t>
+        </is>
+      </c>
+      <c r="O14" s="42" t="inlineStr">
+        <is>
+          <t>37.29</t>
+        </is>
+      </c>
+      <c r="P14" s="42" t="inlineStr">
+        <is>
+          <t>114.59</t>
+        </is>
+      </c>
+      <c r="Q14" s="44" t="inlineStr">
+        <is>
+          <t>119.38</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>124.00</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>129.79</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>134.58</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>122.99</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>105.62</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>92.16</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>81.71</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>73.71</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>67.19</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15.65" customHeight="1">
       <c r="A15" s="11" t="inlineStr">
@@ -7300,18 +8137,111 @@
           <t>49.05</t>
         </is>
       </c>
-      <c r="F15" s="42" t="n"/>
-      <c r="G15" s="42" t="n"/>
-      <c r="H15" s="42" t="n"/>
-      <c r="I15" s="44" t="n"/>
-      <c r="J15" s="42" t="n"/>
-      <c r="K15" s="42" t="n"/>
-      <c r="L15" s="42" t="n"/>
-      <c r="M15" s="42" t="n"/>
-      <c r="N15" s="42" t="n"/>
-      <c r="O15" s="42" t="n"/>
-      <c r="P15" s="42" t="n"/>
-      <c r="Q15" s="44" t="n"/>
+      <c r="F15" s="42" t="inlineStr">
+        <is>
+          <t>44.54</t>
+        </is>
+      </c>
+      <c r="G15" s="42" t="inlineStr">
+        <is>
+          <t>44.39</t>
+        </is>
+      </c>
+      <c r="H15" s="42" t="inlineStr">
+        <is>
+          <t>43.51</t>
+        </is>
+      </c>
+      <c r="I15" s="44" t="inlineStr">
+        <is>
+          <t>42.74</t>
+        </is>
+      </c>
+      <c r="J15" s="42" t="inlineStr">
+        <is>
+          <t>42.09</t>
+        </is>
+      </c>
+      <c r="K15" s="42" t="inlineStr">
+        <is>
+          <t>40.83</t>
+        </is>
+      </c>
+      <c r="L15" s="42" t="inlineStr">
+        <is>
+          <t>40.31</t>
+        </is>
+      </c>
+      <c r="M15" s="42" t="inlineStr">
+        <is>
+          <t>39.76</t>
+        </is>
+      </c>
+      <c r="N15" s="42" t="inlineStr">
+        <is>
+          <t>39.29</t>
+        </is>
+      </c>
+      <c r="O15" s="42" t="inlineStr">
+        <is>
+          <t>38.83</t>
+        </is>
+      </c>
+      <c r="P15" s="42" t="inlineStr">
+        <is>
+          <t>108.69</t>
+        </is>
+      </c>
+      <c r="Q15" s="44" t="inlineStr">
+        <is>
+          <t>113.98</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>118.28</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>122.91</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>127.69</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>118.49</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>103.96</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>91.87</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>82.28</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>74.73</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>68.54</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15.65" customHeight="1">
       <c r="A16" s="11" t="inlineStr">
@@ -7339,18 +8269,111 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="F16" s="42" t="n"/>
-      <c r="G16" s="42" t="n"/>
-      <c r="H16" s="42" t="n"/>
-      <c r="I16" s="44" t="n"/>
-      <c r="J16" s="42" t="n"/>
-      <c r="K16" s="42" t="n"/>
-      <c r="L16" s="42" t="n"/>
-      <c r="M16" s="42" t="n"/>
-      <c r="N16" s="42" t="n"/>
-      <c r="O16" s="42" t="n"/>
-      <c r="P16" s="42" t="n"/>
-      <c r="Q16" s="44" t="n"/>
+      <c r="F16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I16" s="44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="J16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="K16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M16" s="42" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="N16" s="42" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="O16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P16" s="42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q16" s="44" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15.65" customHeight="1">
       <c r="A17" s="11" t="inlineStr">
@@ -7378,18 +8401,111 @@
           <t>50.06</t>
         </is>
       </c>
-      <c r="F17" s="42" t="n"/>
-      <c r="G17" s="42" t="n"/>
-      <c r="H17" s="42" t="n"/>
-      <c r="I17" s="44" t="n"/>
-      <c r="J17" s="42" t="n"/>
-      <c r="K17" s="42" t="n"/>
-      <c r="L17" s="42" t="n"/>
-      <c r="M17" s="42" t="n"/>
-      <c r="N17" s="42" t="n"/>
-      <c r="O17" s="42" t="n"/>
-      <c r="P17" s="42" t="n"/>
-      <c r="Q17" s="44" t="n"/>
+      <c r="F17" s="42" t="inlineStr">
+        <is>
+          <t>48.49</t>
+        </is>
+      </c>
+      <c r="G17" s="42" t="inlineStr">
+        <is>
+          <t>48.41</t>
+        </is>
+      </c>
+      <c r="H17" s="42" t="inlineStr">
+        <is>
+          <t>48.00</t>
+        </is>
+      </c>
+      <c r="I17" s="44" t="inlineStr">
+        <is>
+          <t>47.60</t>
+        </is>
+      </c>
+      <c r="J17" s="42" t="inlineStr">
+        <is>
+          <t>47.20</t>
+        </is>
+      </c>
+      <c r="K17" s="42" t="inlineStr">
+        <is>
+          <t>46.47</t>
+        </is>
+      </c>
+      <c r="L17" s="42" t="inlineStr">
+        <is>
+          <t>46.11</t>
+        </is>
+      </c>
+      <c r="M17" s="42" t="inlineStr">
+        <is>
+          <t>45.75</t>
+        </is>
+      </c>
+      <c r="N17" s="42" t="inlineStr">
+        <is>
+          <t>45.37</t>
+        </is>
+      </c>
+      <c r="O17" s="42" t="inlineStr">
+        <is>
+          <t>45.05</t>
+        </is>
+      </c>
+      <c r="P17" s="42" t="inlineStr">
+        <is>
+          <t>49.56</t>
+        </is>
+      </c>
+      <c r="Q17" s="44" t="inlineStr">
+        <is>
+          <t>50.25</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>50.74</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>51.08</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>51.30</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>51.74</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>51.81</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>51.50</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>51.05</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>50.58</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>50.10</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15" customFormat="1" customHeight="1" s="3">
       <c r="A18" s="11" t="inlineStr">
@@ -7417,18 +8533,111 @@
           <t>0.20</t>
         </is>
       </c>
-      <c r="F18" s="47" t="n"/>
-      <c r="G18" s="47" t="n"/>
-      <c r="H18" s="47" t="n"/>
-      <c r="I18" s="48" t="n"/>
-      <c r="J18" s="47" t="n"/>
-      <c r="K18" s="47" t="n"/>
-      <c r="L18" s="47" t="n"/>
-      <c r="M18" s="47" t="n"/>
-      <c r="N18" s="47" t="n"/>
-      <c r="O18" s="47" t="n"/>
-      <c r="P18" s="47" t="n"/>
-      <c r="Q18" s="48" t="n"/>
+      <c r="F18" s="47" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="G18" s="47" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="H18" s="47" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="I18" s="48" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="J18" s="47" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="K18" s="47" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="L18" s="47" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="M18" s="47" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="N18" s="47" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="O18" s="47" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="P18" s="47" t="inlineStr">
+        <is>
+          <t>421.55</t>
+        </is>
+      </c>
+      <c r="Q18" s="48" t="inlineStr">
+        <is>
+          <t>436.46</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>441.47</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>451.62</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>459.61</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15" customFormat="1" customHeight="1" s="3">
       <c r="A19" s="30" t="n"/>
@@ -8264,7 +9473,11 @@
           <t>2024-04-19 16:39:02</t>
         </is>
       </c>
-      <c r="F6" s="38" t="n"/>
+      <c r="F6" s="38" t="inlineStr">
+        <is>
+          <t>2024-04-19 17:18:44</t>
+        </is>
+      </c>
       <c r="G6" s="38" t="n"/>
       <c r="H6" s="38" t="n"/>
       <c r="I6" s="38" t="n"/>
@@ -8303,7 +9516,11 @@
           <t>20832.00</t>
         </is>
       </c>
-      <c r="F7" s="39" t="n"/>
+      <c r="F7" s="39" t="inlineStr">
+        <is>
+          <t>20832.00</t>
+        </is>
+      </c>
       <c r="G7" s="39" t="n"/>
       <c r="H7" s="39" t="n"/>
       <c r="I7" s="39" t="n"/>
@@ -8342,7 +9559,11 @@
           <t>480.40</t>
         </is>
       </c>
-      <c r="F8" s="40" t="n"/>
+      <c r="F8" s="40" t="inlineStr">
+        <is>
+          <t>479.10</t>
+        </is>
+      </c>
       <c r="G8" s="40" t="n"/>
       <c r="H8" s="40" t="n"/>
       <c r="I8" s="41" t="n"/>
@@ -8381,7 +9602,11 @@
           <t>480.52</t>
         </is>
       </c>
-      <c r="F9" s="43" t="n"/>
+      <c r="F9" s="43" t="inlineStr">
+        <is>
+          <t>479.21</t>
+        </is>
+      </c>
       <c r="G9" s="43" t="n"/>
       <c r="H9" s="43" t="n"/>
       <c r="I9" s="44" t="n"/>
@@ -8420,7 +9645,11 @@
           <t>480.96</t>
         </is>
       </c>
-      <c r="F10" s="47" t="n"/>
+      <c r="F10" s="47" t="inlineStr">
+        <is>
+          <t>479.66</t>
+        </is>
+      </c>
       <c r="G10" s="47" t="n"/>
       <c r="H10" s="47" t="n"/>
       <c r="I10" s="44" t="n"/>
@@ -8459,7 +9688,11 @@
           <t>-0.58</t>
         </is>
       </c>
-      <c r="F11" s="47" t="n"/>
+      <c r="F11" s="47" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
       <c r="G11" s="47" t="n"/>
       <c r="H11" s="47" t="n"/>
       <c r="I11" s="44" t="n"/>
@@ -8498,7 +9731,11 @@
           <t>35.08</t>
         </is>
       </c>
-      <c r="F12" s="42" t="n"/>
+      <c r="F12" s="42" t="inlineStr">
+        <is>
+          <t>35.07</t>
+        </is>
+      </c>
       <c r="G12" s="42" t="n"/>
       <c r="H12" s="42" t="n"/>
       <c r="I12" s="44" t="n"/>
@@ -8537,7 +9774,11 @@
           <t>35.95</t>
         </is>
       </c>
-      <c r="F13" s="42" t="n"/>
+      <c r="F13" s="42" t="inlineStr">
+        <is>
+          <t>35.95</t>
+        </is>
+      </c>
       <c r="G13" s="42" t="n"/>
       <c r="H13" s="42" t="n"/>
       <c r="I13" s="44" t="n"/>
@@ -8576,7 +9817,11 @@
           <t>36.17</t>
         </is>
       </c>
-      <c r="F14" s="42" t="n"/>
+      <c r="F14" s="42" t="inlineStr">
+        <is>
+          <t>36.07</t>
+        </is>
+      </c>
       <c r="G14" s="42" t="n"/>
       <c r="H14" s="42" t="n"/>
       <c r="I14" s="44" t="n"/>
@@ -8615,7 +9860,11 @@
           <t>35.81</t>
         </is>
       </c>
-      <c r="F15" s="42" t="n"/>
+      <c r="F15" s="42" t="inlineStr">
+        <is>
+          <t>35.75</t>
+        </is>
+      </c>
       <c r="G15" s="42" t="n"/>
       <c r="H15" s="42" t="n"/>
       <c r="I15" s="44" t="n"/>
@@ -8654,7 +9903,11 @@
           <t>-0.01</t>
         </is>
       </c>
-      <c r="F16" s="42" t="n"/>
+      <c r="F16" s="42" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
       <c r="G16" s="42" t="n"/>
       <c r="H16" s="42" t="n"/>
       <c r="I16" s="44" t="n"/>
@@ -8693,7 +9946,11 @@
           <t>35.90</t>
         </is>
       </c>
-      <c r="F17" s="42" t="n"/>
+      <c r="F17" s="42" t="inlineStr">
+        <is>
+          <t>35.82</t>
+        </is>
+      </c>
       <c r="G17" s="42" t="n"/>
       <c r="H17" s="42" t="n"/>
       <c r="I17" s="44" t="n"/>
@@ -8732,7 +9989,11 @@
           <t>-0.18</t>
         </is>
       </c>
-      <c r="F18" s="47" t="n"/>
+      <c r="F18" s="47" t="inlineStr">
+        <is>
+          <t>-0.20</t>
+        </is>
+      </c>
       <c r="G18" s="47" t="n"/>
       <c r="H18" s="47" t="n"/>
       <c r="I18" s="48" t="n"/>

</xml_diff>